<commit_message>
Updates to I.O Spreadsheet
</commit_message>
<xml_diff>
--- a/ECUPrototypeIO/ECUPrototypeIO/Drive-By-Wire-I.O.xlsx
+++ b/ECUPrototypeIO/ECUPrototypeIO/Drive-By-Wire-I.O.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sleven/Documents/SVC-Circuits/ECUPrototypeIO/ECUPrototypeIO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3CBB22F-EFB7-2D46-8CD3-7E74307B01FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF513DA-EADD-714E-A206-3C3E61181D5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{C3E43CB0-A3B5-054E-A962-3CD07BDEA7C6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Signal Name</t>
   </si>
@@ -47,18 +47,12 @@
     <t>Main Relay</t>
   </si>
   <si>
-    <t>Associated Relay(s)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Function </t>
   </si>
   <si>
     <t>SafetyLight1Enable</t>
   </si>
   <si>
-    <t>GPIO</t>
-  </si>
-  <si>
     <t>SafetyLight2Enable</t>
   </si>
   <si>
@@ -93,6 +87,84 @@
   </si>
   <si>
     <t>PWM</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Turns on Safety Lights 2</t>
+  </si>
+  <si>
+    <t>Switching Mosfet (Mosfet A)</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>RC Filter and Non-Inverting OP Amp</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Controls Acceleration of GEM through conversion of PWM to boosted Analog signal</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Failsafe signal to car to allow command of acceleration </t>
+  </si>
+  <si>
+    <t>Failsafe signal to car to allow command of steering motor</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Test and Validate OP-Amp Gain</t>
+  </si>
+  <si>
+    <t>Controls Direction of motor rotation (CCW or CW)</t>
+  </si>
+  <si>
+    <t>Confirm Relay State for CW and CCW</t>
+  </si>
+  <si>
+    <t>Confirm Mosfet state for Enable On/Off</t>
+  </si>
+  <si>
+    <t>ESTOP</t>
+  </si>
+  <si>
+    <t>GPI</t>
+  </si>
+  <si>
+    <t>GPO</t>
+  </si>
+  <si>
+    <t>Secondary Relay(s)</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Detect State of ESTOPs and Drive 'SafetyLight Enable1' to low if low signal is sent</t>
+  </si>
+  <si>
+    <t>Control Duty Cycle to Steering Driver</t>
+  </si>
+  <si>
+    <t>Voltage Divider</t>
+  </si>
+  <si>
+    <t>V-Divder was inverted by mistake (To be fixed)</t>
   </si>
 </sst>
 </file>
@@ -453,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A4A3FC-1EC0-2741-962A-92D3E7A482BA}">
-  <dimension ref="B3:H10"/>
+  <dimension ref="B3:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,8 +538,8 @@
     <col min="4" max="4" width="34.1640625" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" customWidth="1"/>
-    <col min="7" max="7" width="45.6640625" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="70" customWidth="1"/>
+    <col min="8" max="8" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
@@ -484,84 +556,188 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>